<commit_message>
updated task allocation file
</commit_message>
<xml_diff>
--- a/Task Allocation.xlsx
+++ b/Task Allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FrontEnd\API\Capstone\TheStore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E05501D-C106-45FF-8D20-81FB870F1BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC54AB69-0259-4441-8A53-16450778EEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -119,38 +119,30 @@
     <t>Shopping Cart - Increase/Decrease Quantity Buttons</t>
   </si>
   <si>
-    <t>Body - Add New Product Button</t>
-  </si>
-  <si>
-    <t>Body - Product Filter (Search Box)</t>
-  </si>
-  <si>
-    <t>Body - Product Sort by Price Buttons</t>
-  </si>
-  <si>
-    <t>Product List - Edit / Remove Buttons</t>
-  </si>
-  <si>
-    <t>Product List - Product Table</t>
-  </si>
-  <si>
     <t>Admin Page</t>
   </si>
   <si>
-    <t>Product API: https://65a9efbb081bd82e1d95bdd2.mockapi.io/product</t>
-  </si>
-  <si>
     <t>Cart API: https://65a9efbb081bd82e1d95bdd2.mockapi.io/cart</t>
+  </si>
+  <si>
+    <t>Trung</t>
+  </si>
+  <si>
+    <t>Product API: https://65a5f64474cf4207b4ef0e03.mockapi.io/PhoneProducts/</t>
+  </si>
+  <si>
+    <t>Quân</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
+    <numFmt numFmtId="168" formatCode="[$-409]d/mmm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +173,12 @@
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -227,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -425,11 +423,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -476,12 +498,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -494,6 +510,9 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -512,8 +531,26 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,8 +772,8 @@
   </sheetPr>
   <dimension ref="A1:K992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -785,16 +822,18 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="10"/>
+      <c r="F2" s="27" t="s">
+        <v>27</v>
+      </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="13"/>
@@ -802,14 +841,18 @@
       <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="33">
+        <v>45310</v>
+      </c>
+      <c r="D3" s="33">
+        <v>45311</v>
+      </c>
       <c r="E3" s="13"/>
-      <c r="F3" s="10"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="13"/>
@@ -817,14 +860,18 @@
       <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="C4" s="33">
+        <v>45315</v>
+      </c>
+      <c r="D4" s="33">
+        <v>45317</v>
+      </c>
       <c r="E4" s="13"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="28"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="13"/>
@@ -832,14 +879,14 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" ht="23.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="13"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="13"/>
@@ -847,14 +894,14 @@
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="13"/>
@@ -862,14 +909,14 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
       <c r="E7" s="13"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="13"/>
@@ -877,14 +924,14 @@
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="13"/>
@@ -892,14 +939,14 @@
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="10"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="13"/>
@@ -907,14 +954,14 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="10"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="13"/>
@@ -922,14 +969,18 @@
       <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="C11" s="33">
+        <v>45313</v>
+      </c>
+      <c r="D11" s="33">
+        <v>45313</v>
+      </c>
       <c r="E11" s="13"/>
-      <c r="F11" s="10"/>
+      <c r="F11" s="28"/>
       <c r="G11" s="14"/>
       <c r="H11" s="8"/>
       <c r="I11" s="13"/>
@@ -937,14 +988,18 @@
       <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="C12" s="33">
+        <v>45314</v>
+      </c>
+      <c r="D12" s="33">
+        <v>45315</v>
+      </c>
       <c r="E12" s="13"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="14"/>
       <c r="H12" s="8"/>
       <c r="I12" s="13"/>
@@ -952,14 +1007,18 @@
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="19" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="C13" s="33">
+        <v>45314</v>
+      </c>
+      <c r="D13" s="33">
+        <v>45315</v>
+      </c>
       <c r="E13" s="13"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="28"/>
       <c r="G13" s="14"/>
       <c r="H13" s="8"/>
       <c r="I13" s="13"/>
@@ -967,14 +1026,14 @@
       <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="10"/>
+      <c r="F14" s="28"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="13"/>
@@ -982,14 +1041,18 @@
       <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="33">
+        <v>45315</v>
+      </c>
+      <c r="D15" s="33">
+        <v>45317</v>
+      </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="10"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="13"/>
@@ -997,14 +1060,18 @@
       <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="C16" s="33">
+        <v>45315</v>
+      </c>
+      <c r="D16" s="33">
+        <v>45317</v>
+      </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="10"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="13"/>
@@ -1024,16 +1091,18 @@
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="20" t="s">
+      <c r="A18" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="16"/>
+      <c r="F18" s="30" t="s">
+        <v>29</v>
+      </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="13"/>
@@ -1041,14 +1110,12 @@
       <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="21" t="s">
-        <v>11</v>
-      </c>
+      <c r="A19" s="25"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="13"/>
-      <c r="F19" s="17"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="13"/>
@@ -1056,14 +1123,14 @@
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="20" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="10"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="13"/>
@@ -1071,14 +1138,12 @@
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="A21" s="25"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="10"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="14"/>
       <c r="H21" s="8"/>
       <c r="I21" s="13"/>
@@ -1086,14 +1151,12 @@
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="21" t="s">
-        <v>26</v>
-      </c>
+      <c r="A22" s="25"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="10"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="14"/>
       <c r="H22" s="8"/>
       <c r="I22" s="13"/>
@@ -1101,14 +1164,12 @@
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="21" t="s">
-        <v>27</v>
-      </c>
+      <c r="A23" s="25"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="13"/>
-      <c r="F23" s="10"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="14"/>
       <c r="H23" s="8"/>
       <c r="I23" s="13"/>
@@ -1116,14 +1177,12 @@
       <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="21" t="s">
-        <v>13</v>
-      </c>
+      <c r="A24" s="25"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="13"/>
-      <c r="F24" s="10"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="14"/>
       <c r="H24" s="8"/>
       <c r="I24" s="13"/>
@@ -1131,14 +1190,12 @@
       <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="A25" s="25"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="13"/>
-      <c r="F25" s="10"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="14"/>
       <c r="H25" s="8"/>
       <c r="I25" s="13"/>
@@ -1146,14 +1203,12 @@
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="21" t="s">
-        <v>29</v>
-      </c>
+      <c r="A26" s="25"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="13"/>
-      <c r="F26" s="10"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="14"/>
       <c r="H26" s="8"/>
       <c r="I26" s="13"/>
@@ -1161,14 +1216,12 @@
       <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="21" t="s">
-        <v>28</v>
-      </c>
+      <c r="A27" s="26"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="13"/>
-      <c r="F27" s="10"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="14"/>
       <c r="H27" s="8"/>
       <c r="I27" s="13"/>
@@ -1188,8 +1241,8 @@
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
-        <v>31</v>
+      <c r="B29" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
@@ -1202,8 +1255,8 @@
       <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
-        <v>32</v>
+      <c r="B30" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
@@ -2178,11 +2231,13 @@
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A18:A27"/>
+    <mergeCell ref="F2:F16"/>
+    <mergeCell ref="F18:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>